<commit_message>
modificacion del MRD:: se elimino el MER antiguo
</commit_message>
<xml_diff>
--- a/Informacion/MRD-PROYTECTO.xlsx
+++ b/Informacion/MRD-PROYTECTO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="59">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -54,12 +54,6 @@
     <t>PK</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
     <t>AUTOINCREMENT</t>
   </si>
   <si>
@@ -84,15 +78,9 @@
     <t>NULL</t>
   </si>
   <si>
-    <t>blob</t>
-  </si>
-  <si>
     <t>CUENTAS</t>
   </si>
   <si>
-    <t>VIDEOS</t>
-  </si>
-  <si>
     <t>FK (SITIOS DE INTERES)</t>
   </si>
   <si>
@@ -126,12 +114,6 @@
     <t>infoAdicional</t>
   </si>
   <si>
-    <t>dateTime</t>
-  </si>
-  <si>
-    <t>MediumText</t>
-  </si>
-  <si>
     <t>IMAGENES</t>
   </si>
   <si>
@@ -153,12 +135,6 @@
     <t>nombreimagen</t>
   </si>
   <si>
-    <t>nombrevideo</t>
-  </si>
-  <si>
-    <t>video</t>
-  </si>
-  <si>
     <t>idContenido</t>
   </si>
   <si>
@@ -171,24 +147,6 @@
     <t>idComentario</t>
   </si>
   <si>
-    <t>LOCALES</t>
-  </si>
-  <si>
-    <t>idLocal</t>
-  </si>
-  <si>
-    <t>numeroLocal</t>
-  </si>
-  <si>
-    <t>idCategoriap</t>
-  </si>
-  <si>
-    <t>idSitioin</t>
-  </si>
-  <si>
-    <t>FK(Categoria)</t>
-  </si>
-  <si>
     <t>CATEGORIAS</t>
   </si>
   <si>
@@ -220,13 +178,31 @@
   </si>
   <si>
     <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>int(10)</t>
+  </si>
+  <si>
+    <t>int(2)</t>
+  </si>
+  <si>
+    <t>idCategoriaS</t>
+  </si>
+  <si>
+    <t>FK (contenidos_multimedia)</t>
+  </si>
+  <si>
+    <t>longblob</t>
+  </si>
+  <si>
+    <t>FK (sitios_interes)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -246,15 +222,6 @@
       <u/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -313,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -343,9 +310,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -617,7 +581,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -625,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -640,7 +604,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -655,19 +619,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="G2"/>
       <c r="H2"/>
@@ -748,7 +712,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -760,16 +724,16 @@
         <v>0</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -777,13 +741,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>6</v>
@@ -815,10 +779,10 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -826,7 +790,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -844,7 +808,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -853,6 +817,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
       <c r="J16" s="6"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -860,25 +825,28 @@
         <v>0</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>34</v>
+      <c r="H17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="J17" s="6"/>
     </row>
@@ -887,7 +855,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>8</v>
@@ -896,16 +864,19 @@
         <v>8</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="8" t="s">
-        <v>36</v>
+      <c r="I18" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="J18" s="6"/>
     </row>
@@ -928,15 +899,18 @@
       <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>20</v>
+      <c r="G19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
@@ -949,6 +923,9 @@
       <c r="F20" s="1"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
+      <c r="I20" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -956,7 +933,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -964,6 +941,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="9"/>
       <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -971,7 +949,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -986,22 +964,22 @@
         <v>0</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1009,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>8</v>
@@ -1021,10 +999,10 @@
         <v>7</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1038,7 +1016,7 @@
         <v>9</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>9</v>
@@ -1062,7 +1040,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1070,7 +1048,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1078,389 +1056,209 @@
       <c r="F28" s="1"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-    </row>
     <row r="31" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>62</v>
-      </c>
+      <c r="A31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="B33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="B49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="8"/>
-    </row>
-    <row r="37" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49" s="1"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-    </row>
-    <row r="59" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C62" s="1"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>